<commit_message>
ajustement précision lecture shunt
</commit_message>
<xml_diff>
--- a/Esp32stat.xlsx
+++ b/Esp32stat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugosavard/VScode/electronic load/electronic load/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3130818-E21B-4B4C-9AC6-61E0431C2099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D14B17-CBD7-3A4B-899E-A209E2575F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10160" yWindow="500" windowWidth="15420" windowHeight="15720" xr2:uid="{4DB01152-5073-C849-BD41-46FA440F4C8B}"/>
+    <workbookView xWindow="4480" yWindow="500" windowWidth="21100" windowHeight="15720" xr2:uid="{4DB01152-5073-C849-BD41-46FA440F4C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>tension désiré</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>valeur de référence</t>
+  </si>
+  <si>
+    <t>mesure vrai tension sur esp32</t>
+  </si>
+  <si>
+    <t>mv</t>
   </si>
 </sst>
 </file>
@@ -1640,7 +1646,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="fr-FR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -2461,7 +2467,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="fr-FR"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -4830,6 +4836,1231 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-CA"/>
+              <a:t>Mesure prise par l'adc</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-CA" baseline="0"/>
+              <a:t> de l'esp32 s2</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.25163485920192186"/>
+          <c:y val="4.4299517647164083E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="3175" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:alpha val="80000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$BB$6:$BB$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>578</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>679</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>813</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>846</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>913</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>947</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>996</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1034</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1066</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1148</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1313</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1483</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1643</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1810</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2141</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2305</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2478</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2650</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2664</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2663</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$BA$6:$BA$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>458</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>524</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>589</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>688</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>788</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>819</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>854</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>886</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>919</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>952</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>985</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1001</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1034</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1066</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1147</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1311</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1475</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1634</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1796</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1958</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2122</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2284</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2446</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2608</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2771</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2932</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4FB1-1C45-AFF8-1BB15B8A3B64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>reference x=y</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="6350" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="500"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$BE$6:$BE$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$BF$6:$BF$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4FB1-1C45-AFF8-1BB15B8A3B64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>asymptote</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="50"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="2"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln w="9525">
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4FB1-1C45-AFF8-1BB15B8A3B64}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="6350" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:alpha val="77000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="500"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.34074188834687963"/>
+                  <c:y val="0.24554597098531558"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil1!$BB$9:$BB$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>194</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>341</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>378</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>412</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>445</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>545</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>578</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>609</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>642</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>679</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>713</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>745</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>813</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>846</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>913</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>947</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>996</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1034</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1066</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1148</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1313</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1483</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1643</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1810</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1976</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2141</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2305</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2478</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil1!$BA$9:$BA$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>196</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>212</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>229</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>326</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>424</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>458</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>491</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>524</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>557</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>589</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>655</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>688</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>754</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>788</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>819</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>854</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>886</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>919</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>952</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>985</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1034</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1066</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1147</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1311</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1475</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1634</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1796</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1958</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2122</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2284</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2446</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4FB1-1C45-AFF8-1BB15B8A3B64}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1696861888"/>
+        <c:axId val="1696629232"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1696861888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1696629232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1696629232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1696861888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5030,6 +6261,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7095,6 +8366,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7789,6 +9576,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27610</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47488AA7-7937-8C48-AB0B-9A10763F8FDF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8114,10 +9937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BE1E8E-CB62-6548-9498-E544CEE03636}">
-  <dimension ref="C4:AA149"/>
+  <dimension ref="C4:BF149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA49" zoomScale="125" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="AB66" sqref="AB66"/>
+    <sheetView tabSelected="1" topLeftCell="BC14" zoomScale="150" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="BJ21" sqref="BJ21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8129,9 +9952,11 @@
     <col min="9" max="9" width="9.1640625" customWidth="1"/>
     <col min="10" max="10" width="12.5" customWidth="1"/>
     <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="53" max="53" width="20" customWidth="1"/>
+    <col min="54" max="54" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -8141,8 +9966,11 @@
       <c r="Z4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>3</v>
       </c>
@@ -8155,8 +9983,11 @@
       <c r="Z5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -8175,8 +10006,20 @@
       <c r="S6">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="7" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA6">
+        <v>0</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
+      <c r="BE6">
+        <v>0</v>
+      </c>
+      <c r="BF6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C7">
         <v>0.5</v>
       </c>
@@ -8195,16 +10038,34 @@
       <c r="S7">
         <v>13.27</v>
       </c>
-    </row>
-    <row r="8" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA7">
+        <v>15</v>
+      </c>
+      <c r="BB7">
+        <v>1</v>
+      </c>
+      <c r="BE7">
+        <v>2500</v>
+      </c>
+      <c r="BF7">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="8" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>0.6</v>
       </c>
       <c r="D8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="9" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA8">
+        <v>32</v>
+      </c>
+      <c r="BB8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>0.7</v>
       </c>
@@ -8217,8 +10078,14 @@
       <c r="AA9">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="10" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA9">
+        <v>48</v>
+      </c>
+      <c r="BB9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>0.8</v>
       </c>
@@ -8231,8 +10098,14 @@
       <c r="AA10">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="11" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA10">
+        <v>64</v>
+      </c>
+      <c r="BB10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>0.9</v>
       </c>
@@ -8245,8 +10118,14 @@
       <c r="AA11">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="12" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA11">
+        <v>81</v>
+      </c>
+      <c r="BB11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>1</v>
       </c>
@@ -8265,8 +10144,14 @@
       <c r="AA12">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="13" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA12">
+        <v>97</v>
+      </c>
+      <c r="BB12">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C13">
         <v>1.1000000000000001</v>
       </c>
@@ -8285,8 +10170,14 @@
       <c r="AA13">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="14" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA13">
+        <v>114</v>
+      </c>
+      <c r="BB13">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>1.2</v>
       </c>
@@ -8305,8 +10196,14 @@
       <c r="AA14">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA14">
+        <v>130</v>
+      </c>
+      <c r="BB14">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>1.3</v>
       </c>
@@ -8325,8 +10222,14 @@
       <c r="AA15">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="16" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA15">
+        <v>147</v>
+      </c>
+      <c r="BB15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="3:58" x14ac:dyDescent="0.2">
       <c r="C16">
         <v>1.4</v>
       </c>
@@ -8345,8 +10248,14 @@
       <c r="AA16">
         <v>0.78</v>
       </c>
-    </row>
-    <row r="17" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA16">
+        <v>163</v>
+      </c>
+      <c r="BB16">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C17">
         <v>1.5</v>
       </c>
@@ -8365,8 +10274,14 @@
       <c r="AA17">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="18" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA17">
+        <v>179</v>
+      </c>
+      <c r="BB17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>1.6</v>
       </c>
@@ -8385,8 +10300,14 @@
       <c r="AA18">
         <v>0.98</v>
       </c>
-    </row>
-    <row r="19" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA18">
+        <v>196</v>
+      </c>
+      <c r="BB18">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>1.7</v>
       </c>
@@ -8405,8 +10326,14 @@
       <c r="AA19">
         <v>1.08</v>
       </c>
-    </row>
-    <row r="20" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA19">
+        <v>212</v>
+      </c>
+      <c r="BB19">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C20">
         <v>1.8</v>
       </c>
@@ -8425,8 +10352,14 @@
       <c r="AA20">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="21" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA20">
+        <v>229</v>
+      </c>
+      <c r="BB20">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C21">
         <v>1.9</v>
       </c>
@@ -8445,8 +10378,14 @@
       <c r="AA21">
         <v>1.28</v>
       </c>
-    </row>
-    <row r="22" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA21">
+        <v>245</v>
+      </c>
+      <c r="BB21">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C22">
         <v>2</v>
       </c>
@@ -8465,8 +10404,14 @@
       <c r="AA22">
         <v>1.39</v>
       </c>
-    </row>
-    <row r="23" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA22">
+        <v>262</v>
+      </c>
+      <c r="BB22">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C23">
         <v>2.1</v>
       </c>
@@ -8485,8 +10430,14 @@
       <c r="AA23">
         <v>1.48</v>
       </c>
-    </row>
-    <row r="24" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA23">
+        <v>277</v>
+      </c>
+      <c r="BB23">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C24">
         <v>2.2000000000000002</v>
       </c>
@@ -8505,8 +10456,14 @@
       <c r="AA24">
         <v>1.59</v>
       </c>
-    </row>
-    <row r="25" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA24">
+        <v>294</v>
+      </c>
+      <c r="BB24">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="25" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C25">
         <v>2.2999999999999998</v>
       </c>
@@ -8525,8 +10482,14 @@
       <c r="AA25">
         <v>1.69</v>
       </c>
-    </row>
-    <row r="26" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA25">
+        <v>310</v>
+      </c>
+      <c r="BB25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C26">
         <v>2.4</v>
       </c>
@@ -8545,8 +10508,14 @@
       <c r="AA26">
         <v>1.79</v>
       </c>
-    </row>
-    <row r="27" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA26">
+        <v>326</v>
+      </c>
+      <c r="BB26">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="27" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C27">
         <v>2.5</v>
       </c>
@@ -8565,8 +10534,14 @@
       <c r="AA27">
         <v>1.89</v>
       </c>
-    </row>
-    <row r="28" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA27">
+        <v>358</v>
+      </c>
+      <c r="BB27">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="28" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C28">
         <v>2.6</v>
       </c>
@@ -8585,8 +10560,14 @@
       <c r="AA28">
         <v>1.99</v>
       </c>
-    </row>
-    <row r="29" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA28">
+        <v>391</v>
+      </c>
+      <c r="BB28">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="29" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C29">
         <v>2.7</v>
       </c>
@@ -8605,8 +10586,14 @@
       <c r="AA29">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="30" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA29">
+        <v>424</v>
+      </c>
+      <c r="BB29">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="30" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C30">
         <v>2.8</v>
       </c>
@@ -8625,8 +10612,14 @@
       <c r="AA30">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="31" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA30">
+        <v>458</v>
+      </c>
+      <c r="BB30">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="31" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C31">
         <v>2.9</v>
       </c>
@@ -8645,8 +10638,14 @@
       <c r="AA31">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="32" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA31">
+        <v>491</v>
+      </c>
+      <c r="BB31">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="32" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C32">
         <v>3</v>
       </c>
@@ -8665,8 +10664,14 @@
       <c r="AA32">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="33" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA32">
+        <v>524</v>
+      </c>
+      <c r="BB32">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="33" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C33">
         <v>3.1</v>
       </c>
@@ -8685,8 +10690,14 @@
       <c r="AA33">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="34" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA33">
+        <v>557</v>
+      </c>
+      <c r="BB33">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="34" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C34">
         <v>3.2</v>
       </c>
@@ -8705,8 +10716,14 @@
       <c r="AA34">
         <v>2.6</v>
       </c>
-    </row>
-    <row r="35" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA34">
+        <v>589</v>
+      </c>
+      <c r="BB34">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="35" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C35">
         <v>3.3</v>
       </c>
@@ -8725,8 +10742,14 @@
       <c r="AA35">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="36" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA35">
+        <v>620</v>
+      </c>
+      <c r="BB35">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="36" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C36">
         <v>3.4</v>
       </c>
@@ -8745,8 +10768,14 @@
       <c r="AA36">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="37" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA36">
+        <v>655</v>
+      </c>
+      <c r="BB36">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="37" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C37">
         <v>3.5</v>
       </c>
@@ -8765,8 +10794,14 @@
       <c r="AA37">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="38" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA37">
+        <v>688</v>
+      </c>
+      <c r="BB37">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="38" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C38">
         <v>3.6</v>
       </c>
@@ -8785,8 +10820,14 @@
       <c r="AA38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA38">
+        <v>722</v>
+      </c>
+      <c r="BB38">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="39" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C39">
         <v>3.7</v>
       </c>
@@ -8805,8 +10846,14 @@
       <c r="AA39">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="40" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA39">
+        <v>754</v>
+      </c>
+      <c r="BB39">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="40" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C40">
         <v>3.8</v>
       </c>
@@ -8825,8 +10872,14 @@
       <c r="AA40">
         <v>3.21</v>
       </c>
-    </row>
-    <row r="41" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA40">
+        <v>788</v>
+      </c>
+      <c r="BB40">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="41" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C41">
         <v>3.9</v>
       </c>
@@ -8845,8 +10898,14 @@
       <c r="AA41">
         <v>3.29</v>
       </c>
-    </row>
-    <row r="42" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA41">
+        <v>819</v>
+      </c>
+      <c r="BB41">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="42" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C42">
         <v>4</v>
       </c>
@@ -8865,8 +10924,14 @@
       <c r="AA42">
         <v>3.39</v>
       </c>
-    </row>
-    <row r="43" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA42">
+        <v>854</v>
+      </c>
+      <c r="BB42">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="43" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C43">
         <v>4.0999999999999996</v>
       </c>
@@ -8885,8 +10950,14 @@
       <c r="AA43">
         <v>3.82</v>
       </c>
-    </row>
-    <row r="44" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA43">
+        <v>886</v>
+      </c>
+      <c r="BB43">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="44" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C44">
         <v>4.2</v>
       </c>
@@ -8905,8 +10976,14 @@
       <c r="AA44">
         <v>4.8499999999999996</v>
       </c>
-    </row>
-    <row r="45" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA44">
+        <v>919</v>
+      </c>
+      <c r="BB44">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="45" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C45">
         <v>4.3</v>
       </c>
@@ -8925,8 +11002,14 @@
       <c r="AA45">
         <v>5.86</v>
       </c>
-    </row>
-    <row r="46" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA45">
+        <v>952</v>
+      </c>
+      <c r="BB45">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="46" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C46">
         <v>4.4000000000000004</v>
       </c>
@@ -8945,8 +11028,14 @@
       <c r="AA46">
         <v>6.87</v>
       </c>
-    </row>
-    <row r="47" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA46">
+        <v>985</v>
+      </c>
+      <c r="BB46">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="47" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C47">
         <v>4.5</v>
       </c>
@@ -8965,8 +11054,14 @@
       <c r="AA47">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="48" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA47">
+        <v>1017</v>
+      </c>
+      <c r="BB47">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="48" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C48">
         <v>4.5999999999999996</v>
       </c>
@@ -8985,8 +11080,14 @@
       <c r="AA48">
         <v>8.91</v>
       </c>
-    </row>
-    <row r="49" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA48">
+        <v>1001</v>
+      </c>
+      <c r="BB48">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="49" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C49">
         <v>4.7</v>
       </c>
@@ -9005,8 +11106,14 @@
       <c r="AA49">
         <v>9.93</v>
       </c>
-    </row>
-    <row r="50" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA49">
+        <v>1034</v>
+      </c>
+      <c r="BB49">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="50" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C50">
         <v>4.8</v>
       </c>
@@ -9025,8 +11132,14 @@
       <c r="AA50">
         <v>10.94</v>
       </c>
-    </row>
-    <row r="51" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA50">
+        <v>1066</v>
+      </c>
+      <c r="BB50">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="51" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C51">
         <v>4.9000000000000004</v>
       </c>
@@ -9045,8 +11158,14 @@
       <c r="AA51">
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA51">
+        <v>1147</v>
+      </c>
+      <c r="BB51">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="52" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C52">
         <v>5</v>
       </c>
@@ -9065,8 +11184,14 @@
       <c r="AA52">
         <v>13.02</v>
       </c>
-    </row>
-    <row r="53" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA52">
+        <v>1311</v>
+      </c>
+      <c r="BB52">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="53" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C53">
         <v>5.0999999999999996</v>
       </c>
@@ -9085,8 +11210,14 @@
       <c r="AA53">
         <v>14.04</v>
       </c>
-    </row>
-    <row r="54" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA53">
+        <v>1475</v>
+      </c>
+      <c r="BB53">
+        <v>1483</v>
+      </c>
+    </row>
+    <row r="54" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C54">
         <v>5.2</v>
       </c>
@@ -9105,8 +11236,14 @@
       <c r="AA54">
         <v>15.09</v>
       </c>
-    </row>
-    <row r="55" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA54">
+        <v>1634</v>
+      </c>
+      <c r="BB54">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="55" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C55">
         <v>5.3</v>
       </c>
@@ -9125,8 +11262,14 @@
       <c r="AA55">
         <v>16.100000000000001</v>
       </c>
-    </row>
-    <row r="56" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA55">
+        <v>1796</v>
+      </c>
+      <c r="BB55">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="56" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C56">
         <v>5.4</v>
       </c>
@@ -9145,8 +11288,14 @@
       <c r="AA56">
         <v>17.11</v>
       </c>
-    </row>
-    <row r="57" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA56">
+        <v>1958</v>
+      </c>
+      <c r="BB56">
+        <v>1976</v>
+      </c>
+    </row>
+    <row r="57" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C57">
         <v>5.5</v>
       </c>
@@ -9165,8 +11314,14 @@
       <c r="AA57">
         <v>18.12</v>
       </c>
-    </row>
-    <row r="58" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA57">
+        <v>2122</v>
+      </c>
+      <c r="BB57">
+        <v>2141</v>
+      </c>
+    </row>
+    <row r="58" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C58">
         <v>5.6</v>
       </c>
@@ -9185,8 +11340,14 @@
       <c r="AA58">
         <v>19.170000000000002</v>
       </c>
-    </row>
-    <row r="59" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA58">
+        <v>2284</v>
+      </c>
+      <c r="BB58">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="59" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C59">
         <v>5.7</v>
       </c>
@@ -9205,8 +11366,14 @@
       <c r="AA59">
         <v>20.170000000000002</v>
       </c>
-    </row>
-    <row r="60" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA59">
+        <v>2446</v>
+      </c>
+      <c r="BB59">
+        <v>2478</v>
+      </c>
+    </row>
+    <row r="60" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C60">
         <v>5.8</v>
       </c>
@@ -9225,8 +11392,14 @@
       <c r="AA60">
         <v>21.18</v>
       </c>
-    </row>
-    <row r="61" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA60">
+        <v>2608</v>
+      </c>
+      <c r="BB60">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="61" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C61">
         <v>5.9</v>
       </c>
@@ -9245,8 +11418,14 @@
       <c r="AA61">
         <v>22.18</v>
       </c>
-    </row>
-    <row r="62" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA61">
+        <v>2771</v>
+      </c>
+      <c r="BB61">
+        <v>2664</v>
+      </c>
+    </row>
+    <row r="62" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C62">
         <v>6</v>
       </c>
@@ -9265,8 +11444,14 @@
       <c r="AA62">
         <v>23.23</v>
       </c>
-    </row>
-    <row r="63" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA62">
+        <v>2932</v>
+      </c>
+      <c r="BB62">
+        <v>2663</v>
+      </c>
+    </row>
+    <row r="63" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C63">
         <v>6.1</v>
       </c>
@@ -9285,8 +11470,14 @@
       <c r="AA63">
         <v>24.25</v>
       </c>
-    </row>
-    <row r="64" spans="3:27" x14ac:dyDescent="0.2">
+      <c r="BA63">
+        <v>3096</v>
+      </c>
+      <c r="BB63">
+        <v>2663</v>
+      </c>
+    </row>
+    <row r="64" spans="3:54" x14ac:dyDescent="0.2">
       <c r="C64">
         <v>6.2</v>
       </c>

</xml_diff>